<commit_message>
Added __repr__ to State, Cycle and Rate
</commit_message>
<xml_diff>
--- a/scalcs/samples/samples.xlsx
+++ b/scalcs/samples/samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DCPROGS\SCALCS\scalcs\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E850A70-B285-470A-ABF3-B60C0D27F1E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C76B61-C46B-4007-92F6-4B7C4C002A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8916" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="58">
   <si>
     <t>mectitle</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>k7b</t>
+  </si>
+  <si>
+    <t>constrain</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:H12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE59CC13-DA1A-4026-A931-51508FFF0962}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1161,8 +1164,8 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" s="2">
+        <v>5.0000000000000002E-11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1175,8 +1178,8 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>1</v>
+      <c r="D6" s="2">
+        <v>5.0000000000000002E-11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1189,8 +1192,8 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" s="2">
+        <v>5.0000000000000002E-11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1203,7 +1206,7 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1217,7 +1220,7 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1231,7 +1234,7 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1607,6 +1610,34 @@
       </c>
       <c r="H26" s="2">
         <v>10000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>